<commit_message>
Final parent outcome measurements added
</commit_message>
<xml_diff>
--- a/data/GASY_brief_parent.xlsx
+++ b/data/GASY_brief_parent.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/University of Oregon Courses/Dissertation/Dissertation Clients/GASY/participant_2_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A374912B-8911-AA49-B50F-7DCBE5DD16F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C3E047-D080-DD43-BC32-C25364D5B60C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="980" windowWidth="26840" windowHeight="14760" xr2:uid="{061739A5-0582-EE47-A472-C84BB2AE7FED}"/>
   </bookViews>
@@ -438,7 +438,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -473,6 +473,9 @@
       <c r="C2">
         <v>51</v>
       </c>
+      <c r="D2">
+        <v>54</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -484,6 +487,9 @@
       <c r="C3">
         <v>60</v>
       </c>
+      <c r="D3">
+        <v>60</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -495,6 +501,9 @@
       <c r="C4">
         <v>55</v>
       </c>
+      <c r="D4">
+        <v>57</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -506,6 +515,9 @@
       <c r="C5">
         <v>65</v>
       </c>
+      <c r="D5">
+        <v>58</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -517,6 +529,9 @@
       <c r="C6">
         <v>56</v>
       </c>
+      <c r="D6">
+        <v>56</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -528,6 +543,9 @@
       <c r="C7">
         <v>61</v>
       </c>
+      <c r="D7">
+        <v>57</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -539,6 +557,9 @@
       <c r="C8">
         <v>53</v>
       </c>
+      <c r="D8">
+        <v>49</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -550,6 +571,9 @@
       <c r="C9">
         <v>62</v>
       </c>
+      <c r="D9">
+        <v>53</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -561,6 +585,9 @@
       <c r="C10">
         <v>53</v>
       </c>
+      <c r="D10">
+        <v>53</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -572,6 +599,9 @@
       <c r="C11">
         <v>57</v>
       </c>
+      <c r="D11">
+        <v>49</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -583,6 +613,9 @@
       <c r="C12">
         <v>53</v>
       </c>
+      <c r="D12">
+        <v>50</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -594,6 +627,9 @@
       <c r="C13">
         <v>56</v>
       </c>
+      <c r="D13">
+        <v>51</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -604,6 +640,9 @@
       </c>
       <c r="C14">
         <v>57</v>
+      </c>
+      <c r="D14">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>